<commit_message>
read also cells that are numbers
</commit_message>
<xml_diff>
--- a/pwddatabase.xlsx
+++ b/pwddatabase.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITALSCO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITALSCO\OneDrive - ABB\xlsx_bundle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="1560" xr2:uid="{4EF85716-84AD-401F-BFA9-BCB814BEA302}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9585" windowHeight="1560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,16 +413,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F876BAE3-C06C-4ED5-BDB3-FDF1703C0A9B}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -438,7 +438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -446,7 +446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -462,7 +462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -470,7 +470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -478,7 +478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -494,7 +494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -502,7 +502,13 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>